<commit_message>
update what I did
update what I did
</commit_message>
<xml_diff>
--- a/Ning Solutions/Plan.xlsb.xlsx
+++ b/Ning Solutions/Plan.xlsb.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E19CE94-56A3-4773-9EE9-03A44794FA1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A4EDD8-4BC2-4E4F-B1AF-2D017EA4C3B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,6 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Two sum</t>
   </si>
@@ -182,10 +181,19 @@
     <t>Letter Combinations of a Phone Number</t>
   </si>
   <si>
-    <t>3.1o</t>
-  </si>
-  <si>
     <t>N-Queens</t>
+  </si>
+  <si>
+    <t>Unique Paths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique Paths II    </t>
+  </si>
+  <si>
+    <t>Longest Common Subsequence</t>
+  </si>
+  <si>
+    <t>Triangle</t>
   </si>
 </sst>
 </file>
@@ -228,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -237,6 +245,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -521,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B4D5F69-D771-4159-83B5-65B5E33BA953}">
   <dimension ref="A1:F110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,14 +573,14 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
-        <v>2.15</v>
-      </c>
-      <c r="D2" s="1">
-        <v>2.17</v>
-      </c>
-      <c r="E2" s="1">
-        <v>2.2200000000000002</v>
+      <c r="C2" s="4">
+        <v>43876</v>
+      </c>
+      <c r="D2" s="4">
+        <v>43878</v>
+      </c>
+      <c r="E2" s="4">
+        <v>43883</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -579,14 +590,14 @@
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
-        <v>2.15</v>
-      </c>
-      <c r="D3" s="1">
-        <v>2.17</v>
-      </c>
-      <c r="E3" s="1">
-        <v>2.2200000000000002</v>
+      <c r="C3" s="4">
+        <v>43876</v>
+      </c>
+      <c r="D3" s="4">
+        <v>43878</v>
+      </c>
+      <c r="E3" s="4">
+        <v>43883</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -596,14 +607,14 @@
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1">
-        <v>2.15</v>
-      </c>
-      <c r="D4" s="1">
-        <v>2.17</v>
-      </c>
-      <c r="E4" s="1">
-        <v>2.2200000000000002</v>
+      <c r="C4" s="4">
+        <v>43876</v>
+      </c>
+      <c r="D4" s="4">
+        <v>43878</v>
+      </c>
+      <c r="E4" s="4">
+        <v>43883</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -613,14 +624,14 @@
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1">
-        <v>2.15</v>
-      </c>
-      <c r="D5" s="1">
-        <v>2.17</v>
-      </c>
-      <c r="E5" s="1">
-        <v>2.2200000000000002</v>
+      <c r="C5" s="4">
+        <v>43876</v>
+      </c>
+      <c r="D5" s="4">
+        <v>43878</v>
+      </c>
+      <c r="E5" s="4">
+        <v>43883</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -630,14 +641,14 @@
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1">
-        <v>2.15</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2.17</v>
-      </c>
-      <c r="E6" s="1">
-        <v>2.2200000000000002</v>
+      <c r="C6" s="4">
+        <v>43876</v>
+      </c>
+      <c r="D6" s="4">
+        <v>43878</v>
+      </c>
+      <c r="E6" s="4">
+        <v>43883</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -647,14 +658,14 @@
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1">
-        <v>2.15</v>
-      </c>
-      <c r="D7" s="1">
-        <v>2.17</v>
-      </c>
-      <c r="E7" s="1">
-        <v>2.2200000000000002</v>
+      <c r="C7" s="4">
+        <v>43876</v>
+      </c>
+      <c r="D7" s="4">
+        <v>43878</v>
+      </c>
+      <c r="E7" s="4">
+        <v>43883</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -664,14 +675,14 @@
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1">
-        <v>2.15</v>
-      </c>
-      <c r="D8" s="1">
-        <v>2.17</v>
-      </c>
-      <c r="E8" s="1">
-        <v>2.2200000000000002</v>
+      <c r="C8" s="4">
+        <v>43876</v>
+      </c>
+      <c r="D8" s="4">
+        <v>43878</v>
+      </c>
+      <c r="E8" s="4">
+        <v>43883</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -681,11 +692,11 @@
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1">
-        <v>2.17</v>
-      </c>
-      <c r="D9" s="1">
-        <v>2.1800000000000002</v>
+      <c r="C9" s="4">
+        <v>43878</v>
+      </c>
+      <c r="D9" s="4">
+        <v>43879</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -695,8 +706,8 @@
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="1">
-        <v>2.1800000000000002</v>
+      <c r="C10" s="4">
+        <v>43879</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -706,8 +717,8 @@
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1">
-        <v>2.1800000000000002</v>
+      <c r="C11" s="4">
+        <v>43879</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -717,11 +728,11 @@
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="1">
-        <v>2.25</v>
-      </c>
-      <c r="D12" s="1">
-        <v>2.2599999999999998</v>
+      <c r="C12" s="4">
+        <v>43886</v>
+      </c>
+      <c r="D12" s="4">
+        <v>43887</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -731,14 +742,14 @@
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="1">
-        <v>2.25</v>
-      </c>
-      <c r="D13" s="1">
-        <v>2.2599999999999998</v>
-      </c>
-      <c r="E13" s="1">
-        <v>3.5</v>
+      <c r="C13" s="4">
+        <v>43886</v>
+      </c>
+      <c r="D13" s="4">
+        <v>43887</v>
+      </c>
+      <c r="E13" s="4">
+        <v>43895</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -748,11 +759,11 @@
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="1">
-        <v>2.25</v>
-      </c>
-      <c r="D14" s="1">
-        <v>2.2599999999999998</v>
+      <c r="C14" s="4">
+        <v>43886</v>
+      </c>
+      <c r="D14" s="4">
+        <v>43887</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -762,11 +773,11 @@
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="1">
-        <v>2.25</v>
-      </c>
-      <c r="D15" s="1">
-        <v>2.2599999999999998</v>
+      <c r="C15" s="4">
+        <v>43886</v>
+      </c>
+      <c r="D15" s="4">
+        <v>43887</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -776,14 +787,14 @@
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="1">
-        <v>2.27</v>
-      </c>
-      <c r="D16" s="1">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="E16" s="1">
-        <v>3.8</v>
+      <c r="C16" s="4">
+        <v>43888</v>
+      </c>
+      <c r="D16" s="4">
+        <v>43889</v>
+      </c>
+      <c r="E16" s="4">
+        <v>43898</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -793,14 +804,14 @@
       <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="1">
-        <v>2.27</v>
-      </c>
-      <c r="D17" s="1">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="E17" s="1">
-        <v>3.6</v>
+      <c r="C17" s="4">
+        <v>43888</v>
+      </c>
+      <c r="D17" s="4">
+        <v>43889</v>
+      </c>
+      <c r="E17" s="4">
+        <v>43898</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -810,11 +821,11 @@
       <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="1">
-        <v>2.27</v>
-      </c>
-      <c r="D18" s="1">
-        <v>2.2799999999999998</v>
+      <c r="C18" s="4">
+        <v>43888</v>
+      </c>
+      <c r="D18" s="4">
+        <v>43889</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -824,11 +835,11 @@
       <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="1">
-        <v>2.27</v>
-      </c>
-      <c r="D19" s="1">
-        <v>2.2799999999999998</v>
+      <c r="C19" s="4">
+        <v>43888</v>
+      </c>
+      <c r="D19" s="4">
+        <v>43889</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -838,14 +849,14 @@
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="1">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="D20" s="1">
-        <v>2.29</v>
-      </c>
-      <c r="E20" s="1">
-        <v>3.3</v>
+      <c r="C20" s="4">
+        <v>43889</v>
+      </c>
+      <c r="D20" s="4">
+        <v>43890</v>
+      </c>
+      <c r="E20" s="4">
+        <v>43893</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -855,14 +866,14 @@
       <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="1">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="D21" s="1">
-        <v>2.29</v>
-      </c>
-      <c r="E21" s="1">
-        <v>3.3</v>
+      <c r="C21" s="4">
+        <v>43889</v>
+      </c>
+      <c r="D21" s="4">
+        <v>43890</v>
+      </c>
+      <c r="E21" s="4">
+        <v>43893</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -872,14 +883,14 @@
       <c r="B22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="1">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="D22" s="1">
-        <v>2.29</v>
-      </c>
-      <c r="E22" s="1">
-        <v>3.3</v>
+      <c r="C22" s="4">
+        <v>43889</v>
+      </c>
+      <c r="D22" s="4">
+        <v>43890</v>
+      </c>
+      <c r="E22" s="4">
+        <v>43893</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -889,14 +900,14 @@
       <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="1">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="D23" s="1">
-        <v>2.29</v>
-      </c>
-      <c r="E23" s="1">
-        <v>3.3</v>
+      <c r="C23" s="4">
+        <v>43889</v>
+      </c>
+      <c r="D23" s="4">
+        <v>43890</v>
+      </c>
+      <c r="E23" s="4">
+        <v>43893</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -906,14 +917,14 @@
       <c r="B24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="1">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="D24" s="1">
-        <v>2.29</v>
-      </c>
-      <c r="E24" s="1">
-        <v>3.3</v>
+      <c r="C24" s="4">
+        <v>43889</v>
+      </c>
+      <c r="D24" s="4">
+        <v>43890</v>
+      </c>
+      <c r="E24" s="4">
+        <v>43893</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -923,14 +934,14 @@
       <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="1">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="D25" s="1">
-        <v>2.29</v>
-      </c>
-      <c r="E25" s="1">
-        <v>3.3</v>
+      <c r="C25" s="4">
+        <v>43889</v>
+      </c>
+      <c r="D25" s="4">
+        <v>43890</v>
+      </c>
+      <c r="E25" s="4">
+        <v>43893</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -940,14 +951,14 @@
       <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="1">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="D26" s="1">
-        <v>2.29</v>
-      </c>
-      <c r="E26" s="1">
-        <v>3.3</v>
+      <c r="C26" s="4">
+        <v>43889</v>
+      </c>
+      <c r="D26" s="4">
+        <v>43890</v>
+      </c>
+      <c r="E26" s="4">
+        <v>43893</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -957,14 +968,14 @@
       <c r="B27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="1">
-        <v>3.3</v>
-      </c>
-      <c r="D27" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="E27" s="1">
-        <v>3.8</v>
+      <c r="C27" s="4">
+        <v>43893</v>
+      </c>
+      <c r="D27" s="4">
+        <v>43895</v>
+      </c>
+      <c r="E27" s="4">
+        <v>43898</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -974,8 +985,8 @@
       <c r="B28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="1">
-        <v>3.3</v>
+      <c r="C28" s="4">
+        <v>43893</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -985,8 +996,8 @@
       <c r="B29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="1">
-        <v>3.3</v>
+      <c r="C29" s="4">
+        <v>43893</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -996,8 +1007,8 @@
       <c r="B30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="1">
-        <v>3.3</v>
+      <c r="C30" s="4">
+        <v>43893</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1007,8 +1018,8 @@
       <c r="B31" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="1">
-        <v>3.3</v>
+      <c r="C31" s="4">
+        <v>43893</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1018,8 +1029,8 @@
       <c r="B32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="1">
-        <v>3.3</v>
+      <c r="C32" s="4">
+        <v>43893</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1029,8 +1040,8 @@
       <c r="B33" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="1">
-        <v>3.3</v>
+      <c r="C33" s="4">
+        <v>43893</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1040,8 +1051,8 @@
       <c r="B34" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="1">
-        <v>3.3</v>
+      <c r="C34" s="4">
+        <v>43893</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1051,8 +1062,8 @@
       <c r="B35" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="1">
-        <v>3.4</v>
+      <c r="C35" s="4">
+        <v>43894</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1062,11 +1073,11 @@
       <c r="B36" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="1">
-        <v>3.4</v>
-      </c>
-      <c r="D36">
-        <v>3.8</v>
+      <c r="C36" s="4">
+        <v>43894</v>
+      </c>
+      <c r="D36" s="4">
+        <v>43898</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1076,11 +1087,11 @@
       <c r="B37" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="1">
-        <v>3.4</v>
-      </c>
-      <c r="D37">
-        <v>3.5</v>
+      <c r="C37" s="4">
+        <v>43894</v>
+      </c>
+      <c r="D37" s="4">
+        <v>43895</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1090,11 +1101,11 @@
       <c r="B38" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="1">
-        <v>3.4</v>
-      </c>
-      <c r="D38">
-        <v>3.5</v>
+      <c r="C38" s="4">
+        <v>43894</v>
+      </c>
+      <c r="D38" s="4">
+        <v>43895</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1104,11 +1115,11 @@
       <c r="B39" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C39" s="1">
-        <v>3.8</v>
-      </c>
-      <c r="D39">
-        <v>3.8</v>
+      <c r="C39" s="4">
+        <v>43898</v>
+      </c>
+      <c r="D39" s="4">
+        <v>43898</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1118,8 +1129,11 @@
       <c r="B40" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="1">
-        <v>3.8</v>
+      <c r="C40" s="4">
+        <v>43898</v>
+      </c>
+      <c r="D40" s="4">
+        <v>43905</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1129,8 +1143,11 @@
       <c r="B41" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="1">
-        <v>3.8</v>
+      <c r="C41" s="4">
+        <v>43898</v>
+      </c>
+      <c r="D41" s="4">
+        <v>43905</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1140,8 +1157,11 @@
       <c r="B42" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C42" s="1">
-        <v>3.8</v>
+      <c r="C42" s="4">
+        <v>43898</v>
+      </c>
+      <c r="D42" s="4">
+        <v>43905</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1151,8 +1171,11 @@
       <c r="B43" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C43" s="1">
-        <v>3.8</v>
+      <c r="C43" s="4">
+        <v>43898</v>
+      </c>
+      <c r="D43" s="4">
+        <v>43905</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1162,8 +1185,11 @@
       <c r="B44" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>49</v>
+      <c r="C44" s="4">
+        <v>43900</v>
+      </c>
+      <c r="D44" s="4">
+        <v>43905</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1171,31 +1197,76 @@
         <v>51</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="4">
+        <v>43900</v>
+      </c>
+      <c r="D45" s="4">
+        <v>43905</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>62</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C45" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C46" s="4">
+        <v>43905</v>
+      </c>
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>63</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="4">
+        <v>43905</v>
+      </c>
+      <c r="D47" s="4"/>
+    </row>
+    <row r="48" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>1143</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="4">
+        <v>43905</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>120</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" s="4">
+        <v>43905</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="67" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>